<commit_message>
change textarea to 100, default supporter/reporter
</commit_message>
<xml_diff>
--- a/web/media/breakdown/IPROS-245/Breakdown-IPROS-245.xlsx
+++ b/web/media/breakdown/IPROS-245/Breakdown-IPROS-245.xlsx
@@ -97,8 +97,8 @@
     <xf applyAlignment="1" borderId="1" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
+    <xf borderId="4" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="3" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="4" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf applyAlignment="1" borderId="0" fillId="2" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
@@ -399,7 +399,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B2:F9"/>
+  <dimension ref="B2:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -453,79 +453,79 @@
       </c>
       <c r="D3" s="2" t="inlineStr">
         <is>
-          <t>---</t>
-        </is>
-      </c>
-      <c r="E3" s="2" t="inlineStr">
-        <is>
-          <t>aaaaaaaaaaaaaaaaaaaaaaaaa</t>
-        </is>
-      </c>
+          <t>ARF02</t>
+        </is>
+      </c>
+      <c r="E3" s="2" t="inlineStr"/>
       <c r="F3" s="2" t="n">
-        <v>6.6</v>
+        <v>5.5</v>
       </c>
     </row>
     <row r="4">
       <c r="B4" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="C4" s="2" t="inlineStr">
+      <c r="C4" s="3" t="n"/>
+      <c r="D4" s="2" t="inlineStr">
+        <is>
+          <t>---</t>
+        </is>
+      </c>
+      <c r="E4" s="2" t="inlineStr">
+        <is>
+          <t>aaaaaaaaaaaaaaaaaaaaaaaaa</t>
+        </is>
+      </c>
+      <c r="F4" s="2" t="n">
+        <v>6.6</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="B5" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="C5" s="2" t="inlineStr">
         <is>
           <t>Datebase Impact</t>
         </is>
       </c>
-      <c r="D4" s="2" t="inlineStr">
+      <c r="D5" s="2" t="inlineStr">
         <is>
           <t>---</t>
         </is>
       </c>
-      <c r="E4" s="2" t="inlineStr">
+      <c r="E5" s="2" t="inlineStr">
         <is>
           <t>11111111111111
 111111111111
 1111111111111111</t>
         </is>
       </c>
-      <c r="F4" s="2" t="n">
+      <c r="F5" s="2" t="n">
         <v>4</v>
       </c>
     </row>
-    <row r="5">
-      <c r="B5" s="2" t="n">
-        <v>3</v>
-      </c>
-      <c r="C5" s="2" t="inlineStr">
+    <row r="6">
+      <c r="B6" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="C6" s="2" t="inlineStr">
         <is>
           <t>Interface Impact</t>
         </is>
       </c>
-      <c r="D5" s="2" t="inlineStr">
+      <c r="D6" s="2" t="inlineStr">
         <is>
           <t>ARF02</t>
         </is>
       </c>
-      <c r="E5" s="2" t="inlineStr">
+      <c r="E6" s="2" t="inlineStr">
         <is>
           <t>222222222222
 22222222222
 2222222222222</t>
         </is>
       </c>
-      <c r="F5" s="2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="B6" s="2" t="n">
-        <v>4</v>
-      </c>
-      <c r="C6" s="3" t="n"/>
-      <c r="D6" s="4" t="n"/>
-      <c r="E6" s="2" t="inlineStr">
-        <is>
-          <t>ccccccccccccccccccccccccc</t>
-        </is>
-      </c>
       <c r="F6" s="2" t="n">
         <v>0</v>
       </c>
@@ -535,37 +535,52 @@
         <v>5</v>
       </c>
       <c r="C7" s="4" t="n"/>
-      <c r="D7" s="2" t="inlineStr">
+      <c r="D7" s="3" t="n"/>
+      <c r="E7" s="2" t="inlineStr">
+        <is>
+          <t>ccccccccccccccccccccccccc</t>
+        </is>
+      </c>
+      <c r="F7" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="B8" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="C8" s="3" t="n"/>
+      <c r="D8" s="2" t="inlineStr">
         <is>
           <t>ARF06</t>
         </is>
       </c>
-      <c r="E7" s="2" t="inlineStr">
+      <c r="E8" s="2" t="inlineStr">
         <is>
           <t>3333333333333
 3333333333333
 3333333333333333333</t>
         </is>
       </c>
-      <c r="F7" s="2" t="n">
+      <c r="F8" s="2" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="8">
-      <c r="B8" s="2" t="n">
-        <v>6</v>
-      </c>
-      <c r="C8" s="2" t="inlineStr">
+    <row r="9">
+      <c r="B9" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="C9" s="2" t="inlineStr">
         <is>
           <t>Security Impact</t>
         </is>
       </c>
-      <c r="D8" s="2" t="inlineStr">
+      <c r="D9" s="2" t="inlineStr">
         <is>
           <t>---</t>
         </is>
       </c>
-      <c r="E8" s="2" t="inlineStr">
+      <c r="E9" s="2" t="inlineStr">
         <is>
           <t>4444444444444444
 44444444444444
@@ -573,20 +588,21 @@
 44444444444444</t>
         </is>
       </c>
-      <c r="F8" s="2" t="n">
+      <c r="F9" s="2" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="9">
-      <c r="F9" s="5">
-        <f>SUM(F2:F8)</f>
+    <row r="10">
+      <c r="F10" s="5">
+        <f>SUM(F2:F9)</f>
         <v/>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="C5:C7"/>
+  <mergeCells count="3">
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="C6:C8"/>
   </mergeCells>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>